<commit_message>
feat: v0.0.15 + v2.2.9 Range
</commit_message>
<xml_diff>
--- a/docs/03_strategies/DCA_Conditional_Buy_LR_with_TrailingStop/Range/Binance_BTC-USDT_1d/equity_curve.xlsx
+++ b/docs/03_strategies/DCA_Conditional_Buy_LR_with_TrailingStop/Range/Binance_BTC-USDT_1d/equity_curve.xlsx
@@ -400,7 +400,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -408,7 +408,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -416,7 +416,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -424,7 +424,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -432,7 +432,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -440,7 +440,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -448,7 +448,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -456,7 +456,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -464,7 +464,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -472,7 +472,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -480,7 +480,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -488,7 +488,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -496,7 +496,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -504,7 +504,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -512,7 +512,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -520,7 +520,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -528,7 +528,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -544,7 +544,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -552,7 +552,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -560,7 +560,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>1628.93010800744</v>
+        <v>1018.08127144288</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -568,7 +568,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>1712.18654723744</v>
+        <v>1070.11641340288</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -576,973 +576,979 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>1709.81322016744</v>
+        <v>1068.63308776288</v>
       </c>
       <c r="B24">
-        <v>0.001386138136541981</v>
+        <v>0.001386134836753983</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
-        <v>1709.58397388744</v>
+        <v>1068.48980920288</v>
       </c>
       <c r="B25">
-        <v>0.001520029084563723</v>
+        <v>0.00152002546604002</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>1652.32264964744</v>
+        <v>1042.030321115604</v>
       </c>
       <c r="B26">
-        <v>0.03496342012883358</v>
+        <v>0.02624582889815141</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>1581.75404990744</v>
+        <v>1042.030321115604</v>
       </c>
       <c r="B27">
-        <v>0.07617890558738982</v>
+        <v>0.02624582889815141</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>1531.91182616744</v>
+        <v>1042.030321115604</v>
       </c>
       <c r="B28">
-        <v>0.1052891820467038</v>
+        <v>0.02624582889815141</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>1603.05040124744</v>
+        <v>1042.030321115604</v>
       </c>
       <c r="B29">
-        <v>0.06374080334066856</v>
+        <v>0.02624582889815141</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>1630.84023197744</v>
+        <v>1042.030321115604</v>
       </c>
       <c r="B30">
-        <v>0.04751019413816182</v>
+        <v>0.02624582889815141</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>1649.77660277744</v>
+        <v>1042.030321115604</v>
       </c>
       <c r="B31">
-        <v>0.03645043500703604</v>
+        <v>0.02624582889815141</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>1678.47635281744</v>
+        <v>1042.030321115604</v>
       </c>
       <c r="B32">
-        <v>0.01968838878823698</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>0.02624582889815141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33">
-        <v>1647.27373585744</v>
+        <v>1042.030321115604</v>
       </c>
       <c r="B33">
-        <v>0.0379122306998233</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>0.02624582889815141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34">
-        <v>1775.59041563744</v>
+        <v>1042.030321115604</v>
       </c>
       <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="C34" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>0.02624582889815141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35">
-        <v>1851.27623199744</v>
+        <v>1042.030321115604</v>
       </c>
       <c r="B35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>0.02624582889815141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36">
-        <v>1837.66905211744</v>
+        <v>1033.627869891365</v>
       </c>
       <c r="B36">
-        <v>0.007350161820701695</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>0.03409773278356221</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37">
-        <v>1832.08627712744</v>
+        <v>1030.618992461365</v>
       </c>
       <c r="B37">
-        <v>0.01036579767963364</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>0.03690946185557231</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38">
-        <v>1795.39431088744</v>
+        <v>1010.843588781365</v>
       </c>
       <c r="B38">
-        <v>0.03018562013822523</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>0.05538913699401427</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39">
-        <v>1777.04204704744</v>
+        <v>1000.952501901364</v>
       </c>
       <c r="B39">
-        <v>0.04009892401087267</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>0.06463213780786714</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40">
-        <v>1787.13908953744</v>
+        <v>1006.394376831365</v>
       </c>
       <c r="B40">
-        <v>0.03464482574315719</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>0.05954682665681632</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41">
-        <v>1743.493479547217</v>
+        <v>952.7084886913646</v>
       </c>
       <c r="B41">
-        <v>0.05822078336409631</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>0.1097150957045581</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42">
-        <v>1743.493479547217</v>
+        <v>950.3292287013645</v>
       </c>
       <c r="B42">
-        <v>0.05822078336409631</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>0.1119384612750703</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43">
-        <v>1743.493479547217</v>
+        <v>1022.167393841365</v>
       </c>
       <c r="B43">
-        <v>0.05822078336409631</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>0.04480729288979091</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44">
-        <v>1743.493479547217</v>
+        <v>1059.846274081365</v>
       </c>
       <c r="B44">
-        <v>0.05822078336409631</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>0.009597216894241645</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45">
-        <v>1743.493479547217</v>
+        <v>1056.919060741365</v>
       </c>
       <c r="B45">
-        <v>0.05822078336409631</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>0.01233263268951179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46">
-        <v>1743.493479547217</v>
+        <v>1051.408215621364</v>
       </c>
       <c r="B46">
-        <v>0.05822078336409631</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>0.01748239494993353</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47">
-        <v>1743.493479547217</v>
+        <v>1036.590626151364</v>
       </c>
       <c r="B47">
-        <v>0.05822078336409631</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>0.0313291029196594</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48">
-        <v>1743.493479547217</v>
+        <v>1035.519684121364</v>
       </c>
       <c r="B48">
-        <v>0.05822078336409631</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
+        <v>0.03232987444001612</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49">
-        <v>1743.493479547217</v>
+        <v>1023.662735261365</v>
       </c>
       <c r="B49">
-        <v>0.05822078336409631</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <v>0.04340992957373357</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50">
-        <v>1743.493479547217</v>
+        <v>1016.494066801364</v>
       </c>
       <c r="B50">
-        <v>0.05822078336409631</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+        <v>0.05010889089253479</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51">
-        <v>1743.493479547217</v>
+        <v>1008.226529731365</v>
       </c>
       <c r="B51">
-        <v>0.05822078336409631</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
+        <v>0.05783472049990401</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52">
-        <v>1743.493479547217</v>
+        <v>1037.398804451364</v>
       </c>
       <c r="B52">
-        <v>0.05822078336409631</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
+        <v>0.03057387826383895</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53">
-        <v>1743.493479547217</v>
+        <v>1022.241864721365</v>
       </c>
       <c r="B53">
-        <v>0.05822078336409631</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
+        <v>0.04473770150789336</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54">
-        <v>1743.493479547217</v>
+        <v>1031.558341061364</v>
       </c>
       <c r="B54">
-        <v>0.05822078336409631</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
+        <v>0.03603166147027326</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55">
-        <v>1743.493479547217</v>
+        <v>1058.452906991365</v>
       </c>
       <c r="B55">
-        <v>0.05822078336409631</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
+        <v>0.01089928746576863</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56">
-        <v>1743.493479547217</v>
+        <v>1030.524211341364</v>
       </c>
       <c r="B56">
-        <v>0.05822078336409631</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
+        <v>0.03699803270526025</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57">
-        <v>1796.834591568857</v>
+        <v>1064.548094641365</v>
       </c>
       <c r="B57">
-        <v>0.02940762674290009</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
+        <v>0.005203470100798357</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58">
-        <v>1795.489395388857</v>
+        <v>1063.716221061364</v>
       </c>
       <c r="B58">
-        <v>0.03013425854249296</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
+        <v>0.005980837469040878</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59">
-        <v>1827.599625058857</v>
+        <v>1083.573288831365</v>
       </c>
       <c r="B59">
-        <v>0.0127893431187398</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
+        <v>0</v>
+      </c>
+      <c r="C59" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60">
-        <v>1830.179172158857</v>
+        <v>1085.168488931365</v>
       </c>
       <c r="B60">
-        <v>0.0113959545711988</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61">
-        <v>1820.864064938857</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B61">
-        <v>0.01642767650388388</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
+        <v>0.009774610262632044</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B62">
-        <v>0.03607441416873325</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
+        <v>0.009774610262632044</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
       <c r="A63">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B63">
-        <v>0.03607441416873325</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
+        <v>0.009774610262632044</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B64">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B65">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B66">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B67">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B68">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B69">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B70">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B71">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B72">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B73">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B74">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B75">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B76">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B77">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B78">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B79">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B80">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B81">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B82">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B83">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B84">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B85">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B86">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B87">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B88">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B89">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B90">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91">
-        <v>1784.492526463633</v>
+        <v>1074.561389882771</v>
       </c>
       <c r="B91">
-        <v>0.03607441416873325</v>
+        <v>0.009774610262632044</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92">
-        <v>1787.077054788473</v>
+        <v>1076.176728314891</v>
       </c>
       <c r="B92">
-        <v>0.03467833492341643</v>
+        <v>0.008286050238454745</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93">
-        <v>1745.868452848473</v>
+        <v>1050.421220894891</v>
       </c>
       <c r="B93">
-        <v>0.0569378990164191</v>
+        <v>0.03202015944149939</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94">
-        <v>1753.831748408473</v>
+        <v>1055.398305974891</v>
       </c>
       <c r="B94">
-        <v>0.05263638235328572</v>
+        <v>0.02743369648135463</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95">
-        <v>1778.197454168473</v>
+        <v>1070.626949654891</v>
       </c>
       <c r="B95">
-        <v>0.03947481016926291</v>
+        <v>0.01340025942956879</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96">
-        <v>1723.435860248473</v>
+        <v>1036.400779094892</v>
       </c>
       <c r="B96">
-        <v>0.0690552655186597</v>
+        <v>0.04494021926908132</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97">
-        <v>1732.923975368473</v>
+        <v>1042.330881254891</v>
       </c>
       <c r="B97">
-        <v>0.0639300902714397</v>
+        <v>0.03947553593143693</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98">
-        <v>1680.943489008473</v>
+        <v>1009.842911774891</v>
       </c>
       <c r="B98">
-        <v>0.09200828058230204</v>
+        <v>0.06941371586512923</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99">
-        <v>1648.465303488473</v>
+        <v>989.5439424148913</v>
       </c>
       <c r="B99">
-        <v>0.1095519539459241</v>
+        <v>0.08811953857104815</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100">
-        <v>1722.293423348473</v>
+        <v>1035.686752394891</v>
       </c>
       <c r="B100">
-        <v>0.06967237326317366</v>
+        <v>0.04559820621514843</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101">
-        <v>1713.521392388473</v>
+        <v>1030.204205114891</v>
       </c>
       <c r="B101">
-        <v>0.07441074283135818</v>
+        <v>0.05065046062164968</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102">
-        <v>1684.516058008473</v>
+        <v>1012.075778774891</v>
       </c>
       <c r="B102">
-        <v>0.09007849347746499</v>
+        <v>0.06735609345646631</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103">
-        <v>1675.634101848473</v>
+        <v>1006.524527894891</v>
       </c>
       <c r="B103">
-        <v>0.09487624111041371</v>
+        <v>0.07247165932169575</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104">
-        <v>1708.646209768473</v>
+        <v>1027.157200454891</v>
       </c>
       <c r="B104">
-        <v>0.07704416000365122</v>
+        <v>0.05345832381624049</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105">
-        <v>1696.971368348473</v>
+        <v>1019.860387394891</v>
       </c>
       <c r="B105">
-        <v>0.08335053461064512</v>
+        <v>0.06018245295786873</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106">
-        <v>1723.172039768473</v>
+        <v>1036.235890454891</v>
       </c>
       <c r="B106">
-        <v>0.06919777287409379</v>
+        <v>0.04509216677002881</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107">
-        <v>1737.202421188473</v>
+        <v>1045.004923514891</v>
       </c>
       <c r="B107">
-        <v>0.06161901116500978</v>
+        <v>0.03701136351279888</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108">
-        <v>1723.940730988473</v>
+        <v>1036.716324914891</v>
       </c>
       <c r="B108">
-        <v>0.06878255054977855</v>
+        <v>0.04464943878363736</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109">
-        <v>1715.173411108473</v>
+        <v>1031.236722074891</v>
       </c>
       <c r="B109">
-        <v>0.07351837534375882</v>
+        <v>0.04969897984190774</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110">
-        <v>1695.218061408473</v>
+        <v>1018.764564974891</v>
       </c>
       <c r="B110">
-        <v>0.0842976147436344</v>
+        <v>0.06119227072458178</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111">
-        <v>1740.152342448473</v>
+        <v>1046.848633694891</v>
       </c>
       <c r="B111">
-        <v>0.06002555838415846</v>
+        <v>0.03531235529536003</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112">
-        <v>1795.801189768473</v>
+        <v>1081.629340454891</v>
       </c>
       <c r="B112">
-        <v>0.02996583722630763</v>
+        <v>0.003261381538970598</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113">
-        <v>1781.702497688473</v>
+        <v>1072.817613014891</v>
       </c>
       <c r="B113">
-        <v>0.03758149816135259</v>
+        <v>0.01138152834555328</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114">
-        <v>1766.188126068473</v>
+        <v>1063.121081354891</v>
       </c>
       <c r="B114">
-        <v>0.04596186374475364</v>
+        <v>0.02031703629561221</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115">
-        <v>1732.379845628473</v>
+        <v>1041.990798434891</v>
       </c>
       <c r="B115">
-        <v>0.06422401169202274</v>
+        <v>0.03978892765214115</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116">
-        <v>1723.575622288473</v>
+        <v>1036.488130814891</v>
       </c>
       <c r="B116">
-        <v>0.06897977055060256</v>
+        <v>0.04485972327155574</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117">
-        <v>1725.229211368473</v>
+        <v>1037.521629254891</v>
       </c>
       <c r="B117">
-        <v>0.06808655480493497</v>
+        <v>0.0439073380424031</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118">
-        <v>1701.112407668473</v>
+        <v>1022.448550154891</v>
       </c>
       <c r="B118">
-        <v>0.08111367808517034</v>
+        <v>0.05779741986264053</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119">
-        <v>1695.469319008473</v>
+        <v>1018.921601774891</v>
       </c>
       <c r="B119">
-        <v>0.08416189345274472</v>
+        <v>0.06104755881891755</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120">
-        <v>1702.970143548473</v>
+        <v>1023.609640994891</v>
       </c>
       <c r="B120">
-        <v>0.08011018879065501</v>
+        <v>0.05672745621013586</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121">
-        <v>1720.212696348473</v>
+        <v>1034.386291394891</v>
       </c>
       <c r="B121">
-        <v>0.07079631520335339</v>
+        <v>0.04679660168392996</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122">
-        <v>1704.650428748473</v>
+        <v>1024.659824594891</v>
       </c>
       <c r="B122">
-        <v>0.07920255265783049</v>
+        <v>0.05575969534100644</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123">
-        <v>1696.206603028473</v>
+        <v>1019.382406634891</v>
       </c>
       <c r="B123">
-        <v>0.08376363628979056</v>
+        <v>0.0606229198207342</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124">
-        <v>1711.406902648473</v>
+        <v>1028.882642294891</v>
       </c>
       <c r="B124">
-        <v>0.07555292232000133</v>
+        <v>0.05186830175275525</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125">
-        <v>1733.932146488473</v>
+        <v>1042.960991414891</v>
       </c>
       <c r="B125">
-        <v>0.06338550859174497</v>
+        <v>0.03889487940995939</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126">
-        <v>1716.468172928473</v>
+        <v>1032.045952334891</v>
       </c>
       <c r="B126">
-        <v>0.07281898656664321</v>
+        <v>0.04895326130303201</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127">
-        <v>1700.492115468473</v>
+        <v>1022.060865554891</v>
       </c>
       <c r="B127">
-        <v>0.08144874002205393</v>
+        <v>0.058154677379749</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128">
-        <v>1694.049713568473</v>
+        <v>1018.034343854891</v>
       </c>
       <c r="B128">
-        <v>0.08492871874627128</v>
+        <v>0.06186518108592043</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129">
-        <v>1703.664242668473</v>
+        <v>1024.043455154891</v>
       </c>
       <c r="B129">
-        <v>0.07973525872457232</v>
+        <v>0.05632768957073864</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130">
-        <v>1706.803392308473</v>
+        <v>1026.005433674891</v>
       </c>
       <c r="B130">
-        <v>0.07803959084652001</v>
+        <v>0.05451969519934652</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131">
-        <v>1735.544906208473</v>
+        <v>1043.968971374891</v>
       </c>
       <c r="B131">
-        <v>0.06251434755584717</v>
+        <v>0.03796600986547727</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132">
-        <v>1716.647193968473</v>
+        <v>1032.157841054891</v>
       </c>
       <c r="B132">
-        <v>0.07272228514688417</v>
+        <v>0.04885015407024607</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133">
-        <v>1775.563175268473</v>
+        <v>1068.980516954891</v>
       </c>
       <c r="B133">
-        <v>0.04089776307843396</v>
+        <v>0.01491747331551685</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134">
-        <v>1829.859942628473</v>
+        <v>1102.916169434891</v>
       </c>
       <c r="B134">
-        <v>0.01156839211718286</v>
+        <v>0</v>
+      </c>
+      <c r="C134" s="2">
+        <v>74</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135">
-        <v>1792.447685988473</v>
+        <v>1079.533389914891</v>
       </c>
       <c r="B135">
-        <v>0.03177729233065008</v>
+        <v>0.02120086745303662</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136">
-        <v>1815.746332128473</v>
+        <v>1094.095117934891</v>
       </c>
       <c r="B136">
-        <v>0.01919211150387434</v>
+        <v>0.007997934697538955</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137">
-        <v>1832.849908068473</v>
+        <v>1104.784907354891</v>
       </c>
       <c r="B137">
-        <v>0.009953308755596302</v>
+        <v>0</v>
+      </c>
+      <c r="C137" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138">
-        <v>1818.544713648473</v>
+        <v>1095.844115294891</v>
       </c>
       <c r="B138">
-        <v>0.01768051562659101</v>
+        <v>0.00809278982766537</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139">
-        <v>1807.808162328473</v>
+        <v>1089.133736534891</v>
       </c>
       <c r="B139">
-        <v>0.02348005603791892</v>
+        <v>0.01416671310026518</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140">
-        <v>1807.249114168473</v>
+        <v>1088.784329654891</v>
       </c>
       <c r="B140">
-        <v>0.02378203591014849</v>
+        <v>0.01448297998413917</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141">
-        <v>1781.198412128473</v>
+        <v>1072.502557934891</v>
       </c>
       <c r="B141">
-        <v>0.03785378900119973</v>
+        <v>0.02922048373858677</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142">
-        <v>1785.593849768473</v>
+        <v>1075.249720454891</v>
       </c>
       <c r="B142">
-        <v>0.03547951466869914</v>
+        <v>0.02673387978363484</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143">
-        <v>1859.455732368473</v>
+        <v>1121.413632254891</v>
       </c>
       <c r="B143">
         <v>0</v>
       </c>
       <c r="C143" s="2">
-        <v>108</v>
+        <v>6</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144">
-        <v>1871.300172668473</v>
+        <v>1128.816445154891</v>
       </c>
       <c r="B144">
         <v>0</v>
@@ -1550,303 +1556,303 @@
     </row>
     <row r="145" spans="1:2">
       <c r="A145">
-        <v>1840.380569448473</v>
+        <v>1109.491594694892</v>
       </c>
       <c r="B145">
-        <v>0.01652305903221729</v>
+        <v>0.01711956850287377</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146">
-        <v>1817.870176403016</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B146">
-        <v>0.02855233866048645</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147">
-        <v>1817.870176403016</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B147">
-        <v>0.02855233866048645</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148">
-        <v>1817.870176403016</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B148">
-        <v>0.02855233866048645</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149">
-        <v>1817.870176403016</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B149">
-        <v>0.02855233866048645</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150">
-        <v>1817.870176403016</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B150">
-        <v>0.02855233866048645</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151">
-        <v>1817.870176403016</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B151">
-        <v>0.02855233866048645</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152">
-        <v>1817.870176403016</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B152">
-        <v>0.02855233866048645</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153">
-        <v>1817.870176403016</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B153">
-        <v>0.02855233866048645</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154">
-        <v>1817.870176403016</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B154">
-        <v>0.02855233866048645</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155">
-        <v>1793.997682940336</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B155">
-        <v>0.04130950814689649</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156">
-        <v>1796.790658140336</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B156">
-        <v>0.03981697624806302</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157">
-        <v>1797.530140500336</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B157">
-        <v>0.03942180588961353</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158">
-        <v>1797.551697020336</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B158">
-        <v>0.0394102863481125</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159">
-        <v>1758.145441220336</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B159">
-        <v>0.06046850906168544</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160">
-        <v>1711.382788660336</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B160">
-        <v>0.08545790052490343</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161">
-        <v>1753.150889260336</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B161">
-        <v>0.06313753674251832</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162">
-        <v>1788.407046340336</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B162">
-        <v>0.04429707619271539</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163">
-        <v>1788.017154500336</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B163">
-        <v>0.04450542963899551</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164">
-        <v>1780.818214060336</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B164">
-        <v>0.04835245565071999</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165">
-        <v>1774.860179380336</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B165">
-        <v>0.05153635675168755</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166">
-        <v>1772.068141420336</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B166">
-        <v>0.05302838780089048</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167">
-        <v>1751.835941540336</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B167">
-        <v>0.06384022877408324</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168">
-        <v>1773.356846420336</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B168">
-        <v>0.05233971955897898</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169">
-        <v>1840.942160060336</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B169">
-        <v>0.01622295185536504</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170">
-        <v>1823.484190580336</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B170">
-        <v>0.02555227792233439</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171">
-        <v>1834.297128460336</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B171">
-        <v>0.01977397573547512</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172">
-        <v>1814.845649500336</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B172">
-        <v>0.03016860896647755</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173">
-        <v>1835.511791500336</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B173">
-        <v>0.01912487461437173</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174">
-        <v>1822.451352100335</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B174">
-        <v>0.02610421421512443</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175">
-        <v>1833.942851740336</v>
+        <v>1106.763903022361</v>
       </c>
       <c r="B175">
-        <v>0.01996329689579701</v>
+        <v>0.01953598587900107</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176">
-        <v>1810.294412060336</v>
+        <v>1091.156503151641</v>
       </c>
       <c r="B176">
-        <v>0.03260073477209302</v>
+        <v>0.03336232579255394</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177">
-        <v>1846.608713100336</v>
+        <v>1113.602835871641</v>
       </c>
       <c r="B177">
-        <v>0.01319481498947706</v>
+        <v>0.01347748728196674</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178">
-        <v>1837.654322140336</v>
+        <v>1108.068012591641</v>
       </c>
       <c r="B178">
-        <v>0.01797993235909234</v>
+        <v>0.01838069657144559</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179">
-        <v>1837.554037460336</v>
+        <v>1108.006025351641</v>
       </c>
       <c r="B179">
-        <v>0.01803352326955376</v>
+        <v>0.01843561005207928</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180">
-        <v>1833.576390900336</v>
+        <v>1105.547391271641</v>
       </c>
       <c r="B180">
-        <v>0.02015912910131501</v>
+        <v>0.02061367371384903</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181">
-        <v>1845.271271620336</v>
+        <v>1112.776146231641</v>
       </c>
       <c r="B181">
-        <v>0.01390952741217333</v>
+        <v>0.01420983809378218</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182">
-        <v>1898.213147500336</v>
+        <v>1145.500195071641</v>
       </c>
       <c r="B182">
         <v>0</v>
@@ -1857,7 +1863,7 @@
     </row>
     <row r="183" spans="1:3">
       <c r="A183">
-        <v>1900.879595300336</v>
+        <v>1147.148360471641</v>
       </c>
       <c r="B183">
         <v>0</v>
@@ -1865,234 +1871,234 @@
     </row>
     <row r="184" spans="1:3">
       <c r="A184">
-        <v>1859.002774860336</v>
+        <v>1121.263763551641</v>
       </c>
       <c r="B184">
-        <v>0.02203023302661278</v>
+        <v>0.02256429753284717</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185">
-        <v>1850.320241693539</v>
+        <v>1079.308250511641</v>
       </c>
       <c r="B185">
-        <v>0.02659787275943082</v>
+        <v>0.0591380437767508</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186">
-        <v>1850.320241693539</v>
+        <v>1087.673631311641</v>
       </c>
       <c r="B186">
-        <v>0.02659787275943082</v>
+        <v>0.0518457169180343</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187">
-        <v>1850.320241693539</v>
+        <v>1085.454256391641</v>
       </c>
       <c r="B187">
-        <v>0.02659787275943082</v>
+        <v>0.05378040557424935</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188">
-        <v>1850.320241693539</v>
+        <v>1068.113470831641</v>
       </c>
       <c r="B188">
-        <v>0.02659787275943082</v>
+        <v>0.06889683354252929</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189">
-        <v>1850.320241693539</v>
+        <v>1094.569856591641</v>
       </c>
       <c r="B189">
-        <v>0.02659787275943082</v>
+        <v>0.04583409233866031</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190">
-        <v>1850.320241693539</v>
+        <v>1090.463057111641</v>
       </c>
       <c r="B190">
-        <v>0.02659787275943082</v>
+        <v>0.0494140996171536</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191">
-        <v>1850.320241693539</v>
+        <v>1090.275357431641</v>
       </c>
       <c r="B191">
-        <v>0.02659787275943082</v>
+        <v>0.04957772246356773</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192">
-        <v>1850.320241693539</v>
+        <v>1087.788336671641</v>
       </c>
       <c r="B192">
-        <v>0.02659787275943082</v>
+        <v>0.05174572517855902</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193">
-        <v>1850.320241693539</v>
+        <v>1091.126378511641</v>
       </c>
       <c r="B193">
-        <v>0.02659787275943082</v>
+        <v>0.04883586455806543</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194">
-        <v>1850.320241693539</v>
+        <v>1090.894071191641</v>
       </c>
       <c r="B194">
-        <v>0.02659787275943082</v>
+        <v>0.04903837308094261</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195">
-        <v>1850.320241693539</v>
+        <v>1095.950376151641</v>
       </c>
       <c r="B195">
-        <v>0.02659787275943082</v>
+        <v>0.04463065640345798</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196">
-        <v>1850.320241693539</v>
+        <v>1083.609122191641</v>
       </c>
       <c r="B196">
-        <v>0.02659787275943082</v>
+        <v>0.0553888585552057</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197">
-        <v>1850.320241693539</v>
+        <v>1074.395037591641</v>
       </c>
       <c r="B197">
-        <v>0.02659787275943082</v>
+        <v>0.06342102328428367</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198">
-        <v>1850.320241693539</v>
+        <v>1079.386458711641</v>
       </c>
       <c r="B198">
-        <v>0.02659787275943082</v>
+        <v>0.05906986759074473</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199">
-        <v>1850.320241693539</v>
+        <v>1077.880806031641</v>
       </c>
       <c r="B199">
-        <v>0.02659787275943082</v>
+        <v>0.06038238542355678</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200">
-        <v>1850.320241693539</v>
+        <v>1074.110591471641</v>
       </c>
       <c r="B200">
-        <v>0.02659787275943082</v>
+        <v>0.06366898259783149</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201">
-        <v>1850.320241693539</v>
+        <v>1078.417835671641</v>
       </c>
       <c r="B201">
-        <v>0.02659787275943082</v>
+        <v>0.05991424227964903</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202">
-        <v>1850.320241693539</v>
+        <v>1081.668979511641</v>
       </c>
       <c r="B202">
-        <v>0.02659787275943082</v>
+        <v>0.05708013297694003</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203">
-        <v>1850.320241693539</v>
+        <v>1081.802802431641</v>
       </c>
       <c r="B203">
-        <v>0.02659787275943082</v>
+        <v>0.0569634759475518</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204">
-        <v>1865.332082634389</v>
+        <v>1091.951330191641</v>
       </c>
       <c r="B204">
-        <v>0.01870055986388242</v>
+        <v>0.04811673204789835</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205">
-        <v>1863.573799224389</v>
+        <v>1090.879008871641</v>
       </c>
       <c r="B205">
-        <v>0.01962554396826621</v>
+        <v>0.04905150330935859</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206">
-        <v>1874.858730024389</v>
+        <v>1097.761330471641</v>
       </c>
       <c r="B206">
-        <v>0.01368885506492867</v>
+        <v>0.04305199894082989</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207">
-        <v>1874.186193744389</v>
+        <v>1097.351171911641</v>
       </c>
       <c r="B207">
-        <v>0.01404265773694591</v>
+        <v>0.04340954516077267</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208">
-        <v>1891.689235404389</v>
+        <v>1108.025722231641</v>
       </c>
       <c r="B208">
-        <v>0.004834793281314864</v>
+        <v>0.03410425328413058</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209">
-        <v>1896.479631534389</v>
+        <v>1110.947232991641</v>
       </c>
       <c r="B209">
-        <v>0.002314698825125583</v>
+        <v>0.03155749398021745</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210">
-        <v>1921.405269934389</v>
+        <v>1126.148589791641</v>
       </c>
       <c r="B210">
-        <v>0</v>
-      </c>
-      <c r="C210" s="2">
-        <v>27</v>
+        <v>0.01830606345579056</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211">
-        <v>1969.147746534389</v>
+        <v>1155.265212991641</v>
       </c>
       <c r="B211">
         <v>0</v>
+      </c>
+      <c r="C211" s="2">
+        <v>28</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212">
-        <v>2054.958816294389</v>
+        <v>1207.598664511641</v>
       </c>
       <c r="B212">
         <v>0</v>
@@ -2100,7 +2106,7 @@
     </row>
     <row r="213" spans="1:3">
       <c r="A213">
-        <v>2157.871115784389</v>
+        <v>1270.361613991641</v>
       </c>
       <c r="B213">
         <v>0</v>
@@ -2108,7 +2114,7 @@
     </row>
     <row r="214" spans="1:3">
       <c r="A214">
-        <v>2255.228341594389</v>
+        <v>1329.736700111641</v>
       </c>
       <c r="B214">
         <v>0</v>
@@ -2116,15 +2122,15 @@
     </row>
     <row r="215" spans="1:3">
       <c r="A215">
-        <v>2247.304192374389</v>
+        <v>1324.904012671641</v>
       </c>
       <c r="B215">
-        <v>0.003513679335192199</v>
+        <v>0.003634319064514058</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216">
-        <v>2277.145615024389</v>
+        <v>1343.103350471641</v>
       </c>
       <c r="B216">
         <v>0</v>
@@ -2135,31 +2141,31 @@
     </row>
     <row r="217" spans="1:3">
       <c r="A217">
-        <v>2272.316272584389</v>
+        <v>1340.546904416706</v>
       </c>
       <c r="B217">
-        <v>0.002120787712536432</v>
+        <v>0.001903387445230997</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218">
-        <v>2228.873088644389</v>
+        <v>1318.252347248526</v>
       </c>
       <c r="B218">
-        <v>0.02119869983785938</v>
+        <v>0.01850267383696758</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219">
-        <v>2266.310941564389</v>
+        <v>1336.713716288526</v>
       </c>
       <c r="B219">
-        <v>0.004758006421949457</v>
+        <v>0.004757365976990169</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220">
-        <v>2417.880480984389</v>
+        <v>1411.455748328526</v>
       </c>
       <c r="B220">
         <v>0</v>
@@ -2170,7 +2176,7 @@
     </row>
     <row r="221" spans="1:3">
       <c r="A221">
-        <v>2428.931733924389</v>
+        <v>1416.905346608526</v>
       </c>
       <c r="B221">
         <v>0</v>
@@ -2178,15 +2184,15 @@
     </row>
     <row r="222" spans="1:3">
       <c r="A222">
-        <v>2421.743764954389</v>
+        <v>1413.360812468526</v>
       </c>
       <c r="B222">
-        <v>0.002959312882123033</v>
+        <v>0.0025016026289153</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223">
-        <v>2441.556037824389</v>
+        <v>1423.130648408526</v>
       </c>
       <c r="B223">
         <v>0</v>
@@ -2197,15 +2203,15 @@
     </row>
     <row r="224" spans="1:3">
       <c r="A224">
-        <v>2414.620389864389</v>
+        <v>1421.422077726546</v>
       </c>
       <c r="B224">
-        <v>0.01103216454700007</v>
+        <v>0.001200571910871973</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225">
-        <v>2455.281287414389</v>
+        <v>1439.197023039006</v>
       </c>
       <c r="B225">
         <v>0</v>
@@ -2216,15 +2222,15 @@
     </row>
     <row r="226" spans="1:3">
       <c r="A226">
-        <v>2450.409199024389</v>
+        <v>1436.953547149006</v>
       </c>
       <c r="B226">
-        <v>0.001984330029709214</v>
+        <v>0.001558838612146785</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227">
-        <v>2456.537068434389</v>
+        <v>1439.775279059006</v>
       </c>
       <c r="B227">
         <v>0</v>
@@ -2235,15 +2241,15 @@
     </row>
     <row r="228" spans="1:3">
       <c r="A228">
-        <v>2451.639332474389</v>
+        <v>1437.519993099006</v>
       </c>
       <c r="B228">
-        <v>0.001993756179352824</v>
+        <v>0.001566415254382059</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229">
-        <v>2520.004355174389</v>
+        <v>1469.000390799006</v>
       </c>
       <c r="B229">
         <v>0</v>
@@ -2254,157 +2260,154 @@
     </row>
     <row r="230" spans="1:3">
       <c r="A230">
-        <v>2483.98110461357</v>
+        <v>1428.927073649006</v>
       </c>
       <c r="B230">
-        <v>0.01429491599363797</v>
+        <v>0.02727931006757833</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231">
-        <v>2483.98110461357</v>
+        <v>1442.004757829006</v>
       </c>
       <c r="B231">
-        <v>0.01429491599363797</v>
+        <v>0.01837687255843179</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232">
-        <v>2524.01050058909</v>
+        <v>1468.578727559006</v>
       </c>
       <c r="B232">
-        <v>0</v>
-      </c>
-      <c r="C232" s="2">
-        <v>3</v>
+        <v>0.0002870409311264144</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233">
-        <v>2507.31665546909</v>
+        <v>1457.918171039006</v>
       </c>
       <c r="B233">
-        <v>0.006614015716695398</v>
+        <v>0.007544055011430073</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234">
-        <v>2503.40964362909</v>
+        <v>1447.083607937914</v>
       </c>
       <c r="B234">
-        <v>0.008161953745910222</v>
+        <v>0.01491952146396036</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235">
-        <v>2496.21345386909</v>
+        <v>1447.083607937914</v>
       </c>
       <c r="B235">
-        <v>0.01101304717770091</v>
+        <v>0.01491952146396036</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236">
-        <v>2469.23082458909</v>
+        <v>1447.083607937914</v>
       </c>
       <c r="B236">
-        <v>0.02170342634755873</v>
+        <v>0.01491952146396036</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237">
-        <v>2457.55979114909</v>
+        <v>1447.083607937914</v>
       </c>
       <c r="B237">
-        <v>0.02632742986785941</v>
+        <v>0.01491952146396036</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238">
-        <v>2490.29676938909</v>
+        <v>1447.083607937914</v>
       </c>
       <c r="B238">
-        <v>0.01335720718758171</v>
+        <v>0.01491952146396036</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239">
-        <v>2471.29186922909</v>
+        <v>1447.083607937914</v>
       </c>
       <c r="B239">
-        <v>0.0208868510442789</v>
+        <v>0.01491952146396036</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240">
-        <v>2391.38101082909</v>
+        <v>1447.083607937914</v>
       </c>
       <c r="B240">
-        <v>0.05254712281468132</v>
+        <v>0.01491952146396036</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241">
-        <v>2379.65723546909</v>
+        <v>1447.083607937914</v>
       </c>
       <c r="B241">
-        <v>0.05719202241286592</v>
+        <v>0.01491952146396036</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242">
-        <v>2395.91544602909</v>
+        <v>1447.083607937914</v>
       </c>
       <c r="B242">
-        <v>0.05075060287193878</v>
+        <v>0.01491952146396036</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243">
-        <v>2390.50357706909</v>
+        <v>1447.083607937914</v>
       </c>
       <c r="B243">
-        <v>0.05289475756493112</v>
+        <v>0.01491952146396036</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244">
-        <v>2389.84807034909</v>
+        <v>1447.083607937914</v>
       </c>
       <c r="B244">
-        <v>0.05315446596148754</v>
+        <v>0.01491952146396036</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245">
-        <v>2419.01846186909</v>
+        <v>1447.083607937914</v>
       </c>
       <c r="B245">
-        <v>0.04159730662590189</v>
+        <v>0.01491952146396036</v>
       </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246">
-        <v>2564.51835002909</v>
+        <v>1540.820649012954</v>
       </c>
       <c r="B246">
         <v>0</v>
       </c>
       <c r="C246" s="2">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247">
-        <v>2509.28797034909</v>
+        <v>1504.863168992954</v>
       </c>
       <c r="B247">
-        <v>0.02153635581487401</v>
+        <v>0.0233365771954277</v>
       </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248">
-        <v>2581.36288634909</v>
+        <v>1551.787205492954</v>
       </c>
       <c r="B248">
         <v>0</v>
@@ -2415,7 +2418,7 @@
     </row>
     <row r="249" spans="1:3">
       <c r="A249">
-        <v>2585.60826842909</v>
+        <v>1554.551141612954</v>
       </c>
       <c r="B249">
         <v>0</v>
@@ -2423,168 +2426,165 @@
     </row>
     <row r="250" spans="1:3">
       <c r="A250">
-        <v>2560.93669418909</v>
+        <v>1538.488828752954</v>
       </c>
       <c r="B250">
-        <v>0.009541884028314018</v>
+        <v>0.01033244415705381</v>
       </c>
     </row>
     <row r="251" spans="1:3">
       <c r="A251">
-        <v>2600.00955242909</v>
+        <v>1530.27256564916</v>
       </c>
       <c r="B251">
-        <v>0</v>
-      </c>
-      <c r="C251" s="2">
-        <v>2</v>
+        <v>0.01561774026848861</v>
       </c>
     </row>
     <row r="252" spans="1:3">
       <c r="A252">
-        <v>2573.29337258909</v>
+        <v>1530.27256564916</v>
       </c>
       <c r="B252">
-        <v>0.01027541603262205</v>
+        <v>0.01561774026848861</v>
       </c>
     </row>
     <row r="253" spans="1:3">
       <c r="A253">
-        <v>2554.80287738909</v>
+        <v>1518.413491352871</v>
       </c>
       <c r="B253">
-        <v>0.01738711882722332</v>
+        <v>0.02324635664452201</v>
       </c>
     </row>
     <row r="254" spans="1:3">
       <c r="A254">
-        <v>2538.22616042909</v>
+        <v>1508.615232482871</v>
       </c>
       <c r="B254">
-        <v>0.02376275577229248</v>
+        <v>0.029549307128244</v>
       </c>
     </row>
     <row r="255" spans="1:3">
       <c r="A255">
-        <v>2486.51784506909</v>
+        <v>1478.051191312871</v>
       </c>
       <c r="B255">
-        <v>0.04365049630451123</v>
+        <v>0.04921031431665179</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="A256">
-        <v>2484.58488794909</v>
+        <v>1476.90864817287</v>
       </c>
       <c r="B256">
-        <v>0.04439393861924978</v>
+        <v>0.04994528089923378</v>
       </c>
     </row>
     <row r="257" spans="1:3">
       <c r="A257">
-        <v>2511.83122682909</v>
+        <v>1493.01356703287</v>
       </c>
       <c r="B257">
-        <v>0.03391461601270607</v>
+        <v>0.03958542947402433</v>
       </c>
     </row>
     <row r="258" spans="1:3">
       <c r="A258">
-        <v>2507.53241786909</v>
+        <v>1490.472602912871</v>
       </c>
       <c r="B258">
-        <v>0.03556799799970056</v>
+        <v>0.04121996181714394</v>
       </c>
     </row>
     <row r="259" spans="1:3">
       <c r="A259">
-        <v>2483.52319994909</v>
+        <v>1476.281099672871</v>
       </c>
       <c r="B259">
-        <v>0.04480227865746556</v>
+        <v>0.05034896559200552</v>
       </c>
     </row>
     <row r="260" spans="1:3">
       <c r="A260">
-        <v>2516.90815034909</v>
+        <v>1496.014463472871</v>
       </c>
       <c r="B260">
-        <v>0.03196196029447718</v>
+        <v>0.03765503531736336</v>
       </c>
     </row>
     <row r="261" spans="1:3">
       <c r="A261">
-        <v>2505.69877994909</v>
+        <v>1489.388765922871</v>
       </c>
       <c r="B261">
-        <v>0.03627324076247695</v>
+        <v>0.04191716434782122</v>
       </c>
     </row>
     <row r="262" spans="1:3">
       <c r="A262">
-        <v>2429.60109386909</v>
+        <v>1444.408518662871</v>
       </c>
       <c r="B262">
-        <v>0.06554147403066046</v>
+        <v>0.07085172047527677</v>
       </c>
     </row>
     <row r="263" spans="1:3">
       <c r="A263">
-        <v>2429.06887994909</v>
+        <v>1444.093934672871</v>
       </c>
       <c r="B263">
-        <v>0.06574617094014013</v>
+        <v>0.07105408370513733</v>
       </c>
     </row>
     <row r="264" spans="1:3">
       <c r="A264">
-        <v>2434.79994026909</v>
+        <v>1447.481481962871</v>
       </c>
       <c r="B264">
-        <v>0.06354192506933332</v>
+        <v>0.06887496768938151</v>
       </c>
     </row>
     <row r="265" spans="1:3">
       <c r="A265">
-        <v>2433.41358122909</v>
+        <v>1446.662025082871</v>
       </c>
       <c r="B265">
-        <v>0.06407513812568733</v>
+        <v>0.06940210176562034</v>
       </c>
     </row>
     <row r="266" spans="1:3">
       <c r="A266">
-        <v>2418.88968938909</v>
+        <v>1438.077161602871</v>
       </c>
       <c r="B266">
-        <v>0.06966122984847767</v>
+        <v>0.0749245083627379</v>
       </c>
     </row>
     <row r="267" spans="1:3">
       <c r="A267">
-        <v>2385.15403946909</v>
+        <v>1418.136504362871</v>
       </c>
       <c r="B267">
-        <v>0.08263643214667005</v>
+        <v>0.08775178480686319</v>
       </c>
     </row>
     <row r="268" spans="1:3">
       <c r="A268">
-        <v>2293.14884234909</v>
+        <v>1363.753556222871</v>
       </c>
       <c r="B268">
-        <v>0.1180229164132538</v>
+        <v>0.1227348398407259</v>
       </c>
     </row>
     <row r="269" spans="1:3">
       <c r="A269">
-        <v>2293.14815738909</v>
+        <v>1363.753151352871</v>
       </c>
       <c r="B269">
-        <v>0.1180231798584399</v>
+        <v>0.1227351002824631</v>
       </c>
       <c r="C269" s="2">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>